<commit_message>
Subindo primeiro teste e relatório inicialmente sendo gerado
</commit_message>
<xml_diff>
--- a/src/excel/planilhaDesafio.xlsx
+++ b/src/excel/planilhaDesafio.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="register" sheetId="1" r:id="rId1"/>
@@ -44,16 +44,16 @@
     <t>Silva</t>
   </si>
   <si>
-    <t>vini001</t>
-  </si>
-  <si>
     <t>Larissa</t>
   </si>
   <si>
     <t>Oliveira</t>
   </si>
   <si>
-    <t>lari001</t>
+    <t>vini007</t>
+  </si>
+  <si>
+    <t>lari007</t>
   </si>
 </sst>
 </file>
@@ -374,13 +374,14 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
     <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -406,7 +407,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2">
         <v>1234</v>
@@ -414,10 +415,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -428,5 +429,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>